<commit_message>
Updated test cases & bug metrics for rounds clearing
Co-Authored-By: tohwangting <tohwangting@users.noreply.github.com>
Co-Authored-By: teeyong <teeyong@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPMProject\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783685A1-39A1-4A28-8815-D48926173E5C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478C7F35-94F8-4ADB-8D0B-5D646E96DA1A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>Bug Log</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>Bootstrap proceeds to check file-specific validations after detecting a blank field</t>
+  </si>
+  <si>
+    <t>Rounds Clearing</t>
+  </si>
+  <si>
+    <t>Clicking on "Start Round" in Round 1 does not direct the admin to bootstrap</t>
   </si>
 </sst>
 </file>
@@ -559,21 +565,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -604,7 +595,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -612,6 +602,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1091,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1109,16 +1115,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
@@ -1166,7 +1172,7 @@
         <f t="shared" ref="F3:F200" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="56">
         <f>SUM($F3:$F8)</f>
         <v>27</v>
       </c>
@@ -1195,7 +1201,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="44"/>
+      <c r="G4" s="57"/>
       <c r="H4" s="25"/>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1218,7 +1224,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="44"/>
+      <c r="G5" s="57"/>
       <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1241,7 +1247,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G6" s="44"/>
+      <c r="G6" s="57"/>
       <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1264,7 +1270,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G7" s="44"/>
+      <c r="G7" s="57"/>
       <c r="H7" s="25"/>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1277,7 +1283,7 @@
       <c r="C8" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="46" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="28" t="s">
@@ -1287,7 +1293,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G8" s="45"/>
+      <c r="G8" s="58"/>
       <c r="H8" s="29"/>
     </row>
     <row r="9" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1297,10 +1303,10 @@
       <c r="B9" s="19">
         <v>2</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="43" t="s">
         <v>47</v>
       </c>
       <c r="E9" s="20" t="s">
@@ -1310,9 +1316,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G9" s="43">
+      <c r="G9" s="56">
         <f>SUM(F9:F15)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H9" s="21" t="str">
         <f xml:space="preserve"> IF(G9&lt;10,Instructions!B7,Instructions!B8)</f>
@@ -1326,7 +1332,7 @@
       <c r="B10" s="23">
         <v>2</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="44" t="s">
         <v>44</v>
       </c>
       <c r="D10" s="41" t="s">
@@ -1339,7 +1345,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G10" s="44"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1349,14 +1355,20 @@
       <c r="B11" s="23">
         <v>2</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G11" s="44"/>
+      <c r="C11" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="24">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G11" s="57"/>
       <c r="H11" s="25"/>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1366,14 +1378,14 @@
       <c r="B12" s="23">
         <v>2</v>
       </c>
-      <c r="C12" s="49"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="41"/>
       <c r="E12" s="24"/>
       <c r="F12" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G12" s="44"/>
+      <c r="G12" s="57"/>
       <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1383,14 +1395,14 @@
       <c r="B13" s="23">
         <v>2</v>
       </c>
-      <c r="C13" s="49"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="41"/>
       <c r="E13" s="24"/>
       <c r="F13" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G13" s="44"/>
+      <c r="G13" s="57"/>
       <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1400,14 +1412,14 @@
       <c r="B14" s="23">
         <v>2</v>
       </c>
-      <c r="C14" s="49"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="41"/>
       <c r="E14" s="24"/>
       <c r="F14" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G14" s="44"/>
+      <c r="G14" s="57"/>
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1417,14 +1429,14 @@
       <c r="B15" s="27">
         <v>2</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="28"/>
       <c r="F15" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G15" s="45"/>
+      <c r="G15" s="58"/>
       <c r="H15" s="29"/>
     </row>
     <row r="16" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1434,14 +1446,14 @@
       <c r="B16" s="19">
         <v>3</v>
       </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="43"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="56">
         <f>SUM(F16:F19)</f>
         <v>0</v>
       </c>
@@ -1457,14 +1469,14 @@
       <c r="B17" s="23">
         <v>3</v>
       </c>
-      <c r="C17" s="49"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="41"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G17" s="44"/>
+      <c r="G17" s="57"/>
       <c r="H17" s="25"/>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1474,14 +1486,14 @@
       <c r="B18" s="23">
         <v>3</v>
       </c>
-      <c r="C18" s="49"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="41"/>
       <c r="E18" s="24"/>
       <c r="F18" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G18" s="44"/>
+      <c r="G18" s="57"/>
       <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1491,14 +1503,14 @@
       <c r="B19" s="27">
         <v>3</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="46"/>
       <c r="E19" s="28"/>
       <c r="F19" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G19" s="45"/>
+      <c r="G19" s="58"/>
       <c r="H19" s="29"/>
     </row>
     <row r="20" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1508,14 +1520,14 @@
       <c r="B20" s="19">
         <v>4</v>
       </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G20" s="43">
+      <c r="G20" s="56">
         <f>SUM(F20:F23)</f>
         <v>0</v>
       </c>
@@ -1531,14 +1543,14 @@
       <c r="B21" s="23">
         <v>4</v>
       </c>
-      <c r="C21" s="49"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="41"/>
       <c r="E21" s="24"/>
       <c r="F21" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G21" s="44"/>
+      <c r="G21" s="57"/>
       <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1548,14 +1560,14 @@
       <c r="B22" s="23">
         <v>4</v>
       </c>
-      <c r="C22" s="49"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="41"/>
       <c r="E22" s="24"/>
       <c r="F22" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G22" s="44"/>
+      <c r="G22" s="57"/>
       <c r="H22" s="25"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1565,14 +1577,14 @@
       <c r="B23" s="27">
         <v>4</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="51"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46"/>
       <c r="E23" s="28"/>
       <c r="F23" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G23" s="45"/>
+      <c r="G23" s="58"/>
       <c r="H23" s="29"/>
     </row>
     <row r="24" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1582,14 +1594,14 @@
       <c r="B24" s="19">
         <v>5</v>
       </c>
-      <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G24" s="43">
+      <c r="G24" s="56">
         <f>SUM(F24:F27)</f>
         <v>0</v>
       </c>
@@ -1605,14 +1617,14 @@
       <c r="B25" s="23">
         <v>5</v>
       </c>
-      <c r="C25" s="49"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="41"/>
       <c r="E25" s="24"/>
       <c r="F25" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G25" s="44"/>
+      <c r="G25" s="57"/>
       <c r="H25" s="25"/>
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1622,14 +1634,14 @@
       <c r="B26" s="23">
         <v>5</v>
       </c>
-      <c r="C26" s="49"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="41"/>
       <c r="E26" s="24"/>
       <c r="F26" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G26" s="44"/>
+      <c r="G26" s="57"/>
       <c r="H26" s="25"/>
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1639,14 +1651,14 @@
       <c r="B27" s="27">
         <v>5</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="51"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="46"/>
       <c r="E27" s="28"/>
       <c r="F27" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G27" s="45"/>
+      <c r="G27" s="58"/>
       <c r="H27" s="29"/>
     </row>
     <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -7470,8 +7482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7488,40 +7500,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="52" t="s">
         <v>27</v>
       </c>
     </row>
@@ -7538,7 +7550,7 @@
         <f>'Bug Metrics'!$C3</f>
         <v>UI</v>
       </c>
-      <c r="D3" s="55" t="str">
+      <c r="D3" s="50" t="str">
         <f>'Bug Metrics'!$D3</f>
         <v>Visibility is poor for login page (black text on dark purple background)</v>
       </c>
@@ -7568,7 +7580,7 @@
         <f>'Bug Metrics'!$C4</f>
         <v>ProcessLogin</v>
       </c>
-      <c r="D4" s="55" t="str">
+      <c r="D4" s="50" t="str">
         <f>'Bug Metrics'!$D4</f>
         <v>Failed to redirect to the targeted page</v>
       </c>
@@ -7598,7 +7610,7 @@
         <f>'Bug Metrics'!$C5</f>
         <v>Bootstrap</v>
       </c>
-      <c r="D5" s="55" t="str">
+      <c r="D5" s="50" t="str">
         <f>'Bug Metrics'!$D5</f>
         <v>Checked the wrong columns for pre-requisite.csv</v>
       </c>
@@ -7628,7 +7640,7 @@
         <f>'Bug Metrics'!$C6</f>
         <v>Bootstrap</v>
       </c>
-      <c r="D6" s="55" t="str">
+      <c r="D6" s="50" t="str">
         <f>'Bug Metrics'!$D6</f>
         <v>Bootstrap errors output not sorted accordingly to the JSON requirements</v>
       </c>
@@ -7658,7 +7670,7 @@
         <f>'Bug Metrics'!$C7</f>
         <v>Login (admin)</v>
       </c>
-      <c r="D7" s="55" t="str">
+      <c r="D7" s="50" t="str">
         <f>'Bug Metrics'!$D7</f>
         <v>No logout button in bootstrap.php that admin is directed to</v>
       </c>
@@ -7688,7 +7700,7 @@
         <f>'Bug Metrics'!$C8</f>
         <v>Bootstrap</v>
       </c>
-      <c r="D8" s="55" t="str">
+      <c r="D8" s="50" t="str">
         <f>'Bug Metrics'!$D8</f>
         <v>Bootstrap does not work on AWS after deployment</v>
       </c>
@@ -7698,7 +7710,7 @@
       <c r="F8" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="59"/>
+      <c r="G8" s="53"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7714,7 +7726,7 @@
         <f>'Bug Metrics'!$C9</f>
         <v>Bootstrap Validation</v>
       </c>
-      <c r="D9" s="56" t="str">
+      <c r="D9" s="51" t="str">
         <f>'Bug Metrics'!$D9</f>
         <v>Bootstrap proceeds to check file-specific validations after detecting a blank field</v>
       </c>
@@ -7724,7 +7736,7 @@
       <c r="F9" s="38">
         <v>43743</v>
       </c>
-      <c r="G9" s="59">
+      <c r="G9" s="53">
         <v>43743</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -7744,7 +7756,7 @@
         <f>'Bug Metrics'!$C10</f>
         <v>Bootstrap Validation</v>
       </c>
-      <c r="D10" s="55" t="str">
+      <c r="D10" s="50" t="str">
         <f>'Bug Metrics'!$D10</f>
         <v>Bootstrap does not check for exam start &amp; end time properly</v>
       </c>
@@ -7754,7 +7766,7 @@
       <c r="F10" s="38">
         <v>43743</v>
       </c>
-      <c r="G10" s="59">
+      <c r="G10" s="53">
         <v>43743</v>
       </c>
       <c r="H10" s="6" t="s">
@@ -7769,18 +7781,26 @@
         <f>'Bug Metrics'!$B11</f>
         <v>2</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="6" t="str">
         <f>'Bug Metrics'!$C11</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="55">
+        <v>Rounds Clearing</v>
+      </c>
+      <c r="D11" s="50" t="str">
         <f>'Bug Metrics'!$D11</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="6"/>
+        <v>Clicking on "Start Round" in Round 1 does not direct the admin to bootstrap</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="53">
+        <v>43748</v>
+      </c>
+      <c r="G11" s="53">
+        <v>43748</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
@@ -7795,13 +7815,13 @@
         <f>'Bug Metrics'!$C12</f>
         <v>0</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="50">
         <f>'Bug Metrics'!$D12</f>
         <v>0</v>
       </c>
       <c r="E12" s="37"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7817,13 +7837,13 @@
         <f>'Bug Metrics'!$C13</f>
         <v>0</v>
       </c>
-      <c r="D13" s="55">
+      <c r="D13" s="50">
         <f>'Bug Metrics'!$D13</f>
         <v>0</v>
       </c>
       <c r="E13" s="37"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7839,13 +7859,13 @@
         <f>'Bug Metrics'!$C14</f>
         <v>0</v>
       </c>
-      <c r="D14" s="55">
+      <c r="D14" s="50">
         <f>'Bug Metrics'!$D14</f>
         <v>0</v>
       </c>
       <c r="E14" s="37"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7861,13 +7881,13 @@
         <f>'Bug Metrics'!$C15</f>
         <v>0</v>
       </c>
-      <c r="D15" s="55">
+      <c r="D15" s="50">
         <f>'Bug Metrics'!$D15</f>
         <v>0</v>
       </c>
       <c r="E15" s="37"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7883,13 +7903,13 @@
         <f>'Bug Metrics'!$C16</f>
         <v>0</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="50">
         <f>'Bug Metrics'!$D16</f>
         <v>0</v>
       </c>
       <c r="E16" s="37"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7905,13 +7925,13 @@
         <f>'Bug Metrics'!$C17</f>
         <v>0</v>
       </c>
-      <c r="D17" s="55">
+      <c r="D17" s="50">
         <f>'Bug Metrics'!$D17</f>
         <v>0</v>
       </c>
       <c r="E17" s="37"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7927,13 +7947,13 @@
         <f>'Bug Metrics'!$C18</f>
         <v>0</v>
       </c>
-      <c r="D18" s="55">
+      <c r="D18" s="50">
         <f>'Bug Metrics'!$D18</f>
         <v>0</v>
       </c>
       <c r="E18" s="37"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7949,13 +7969,13 @@
         <f>'Bug Metrics'!$C19</f>
         <v>0</v>
       </c>
-      <c r="D19" s="55">
+      <c r="D19" s="50">
         <f>'Bug Metrics'!$D19</f>
         <v>0</v>
       </c>
       <c r="E19" s="37"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7971,13 +7991,13 @@
         <f>'Bug Metrics'!$C20</f>
         <v>0</v>
       </c>
-      <c r="D20" s="55">
+      <c r="D20" s="50">
         <f>'Bug Metrics'!$D20</f>
         <v>0</v>
       </c>
       <c r="E20" s="37"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -7993,13 +8013,13 @@
         <f>'Bug Metrics'!$C21</f>
         <v>0</v>
       </c>
-      <c r="D21" s="55">
+      <c r="D21" s="50">
         <f>'Bug Metrics'!$D21</f>
         <v>0</v>
       </c>
       <c r="E21" s="37"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -8015,13 +8035,13 @@
         <f>'Bug Metrics'!$C22</f>
         <v>0</v>
       </c>
-      <c r="D22" s="55">
+      <c r="D22" s="50">
         <f>'Bug Metrics'!$D22</f>
         <v>0</v>
       </c>
       <c r="E22" s="37"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -8037,13 +8057,13 @@
         <f>'Bug Metrics'!$C23</f>
         <v>0</v>
       </c>
-      <c r="D23" s="55">
+      <c r="D23" s="50">
         <f>'Bug Metrics'!$D23</f>
         <v>0</v>
       </c>
       <c r="E23" s="37"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Debugging & update bug metrics
Co-Authored-By: teeyong <teeyong@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPMProject\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B80163-10DE-4A67-A8D3-F5B7D5C81E7B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EB252C-7B88-45DF-9BDC-90AD2C8C6BC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2895" windowWidth="24165" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="73">
   <si>
     <t>Severity</t>
   </si>
@@ -1165,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1864,13 +1864,17 @@
         <v>Test Case 115-bootstrap.txt does not work on AWS</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F24" s="48">
         <v>43751</v>
       </c>
-      <c r="G24" s="48"/>
-      <c r="H24" s="46"/>
+      <c r="G24" s="48">
+        <v>43752</v>
+      </c>
+      <c r="H24" s="46" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="46">
@@ -1890,13 +1894,17 @@
         <v>Bid is created as object in one function but as list in another, causing some functions to not work</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F25" s="48">
         <v>43751</v>
       </c>
-      <c r="G25" s="49"/>
-      <c r="H25" s="50"/>
+      <c r="G25" s="49">
+        <v>43752</v>
+      </c>
+      <c r="H25" s="50" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="46">
@@ -12080,7 +12088,7 @@
       <c r="G10" s="57"/>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>9</v>
       </c>
@@ -12333,7 +12341,7 @@
       <c r="G21" s="57"/>
       <c r="H21" s="15"/>
     </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="13">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Updated bm for debugged problems
Co-Authored-By: tayyuliang <tayyuliang@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPMProject\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F25A3A-7B77-4991-A43E-6EDEE5B3AFB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588A786A-99CB-456F-A4A7-943F9C6AF164}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="84">
   <si>
     <t>Severity</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>TY &amp; YL</t>
-  </si>
-  <si>
-    <t>Unresolved</t>
   </si>
   <si>
     <t>31/09/2019</t>
@@ -279,6 +276,12 @@
   </si>
   <si>
     <t>Ben's bid is stored as "Success" although it is lower than the minimum amount</t>
+  </si>
+  <si>
+    <t>Error displayed when trying to add a bid</t>
+  </si>
+  <si>
+    <t>LF &amp; YL</t>
   </si>
 </sst>
 </file>
@@ -730,27 +733,6 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -777,6 +759,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1234,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1460,13 +1463,13 @@
         <v>22</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="48">
         <v>43750</v>
       </c>
       <c r="H8" s="46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1496,7 +1499,7 @@
         <v>43743</v>
       </c>
       <c r="H9" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1526,7 +1529,7 @@
         <v>43743</v>
       </c>
       <c r="H10" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1556,7 +1559,7 @@
         <v>43748</v>
       </c>
       <c r="H11" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1586,7 +1589,7 @@
         <v>43756</v>
       </c>
       <c r="H12" s="46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1616,7 +1619,7 @@
         <v>43749</v>
       </c>
       <c r="H13" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1646,7 +1649,7 @@
         <v>43750</v>
       </c>
       <c r="H14" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1676,7 +1679,7 @@
         <v>43749</v>
       </c>
       <c r="H15" s="46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1706,7 +1709,7 @@
         <v>43750</v>
       </c>
       <c r="H16" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1736,7 +1739,7 @@
         <v>43750</v>
       </c>
       <c r="H17" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
@@ -1766,7 +1769,7 @@
         <v>43751</v>
       </c>
       <c r="H18" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1796,7 +1799,7 @@
         <v>43751</v>
       </c>
       <c r="H19" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1826,7 +1829,7 @@
         <v>43751</v>
       </c>
       <c r="H20" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1855,7 +1858,7 @@
         <v>43751</v>
       </c>
       <c r="H21" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1884,7 +1887,7 @@
         <v>43751</v>
       </c>
       <c r="H22" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -1913,7 +1916,7 @@
         <v>43751</v>
       </c>
       <c r="H23" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -1942,7 +1945,7 @@
         <v>43752</v>
       </c>
       <c r="H24" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1970,7 +1973,7 @@
         <v>43752</v>
       </c>
       <c r="H25" s="50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1998,7 +2001,7 @@
         <v>43791</v>
       </c>
       <c r="H26" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2026,7 +2029,7 @@
         <v>43760</v>
       </c>
       <c r="H27" s="50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2054,7 +2057,7 @@
         <v>43760</v>
       </c>
       <c r="H28" s="50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2082,7 +2085,7 @@
         <v>43760</v>
       </c>
       <c r="H29" s="50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2101,13 +2104,17 @@
         <v>Min Bid Required reflects "14" although the user bidded for 12 and succeeded</v>
       </c>
       <c r="E30" s="34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F30" s="49">
         <v>43761</v>
       </c>
-      <c r="G30" s="49"/>
-      <c r="H30" s="50"/>
+      <c r="G30" s="49">
+        <v>43762</v>
+      </c>
+      <c r="H30" s="50" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="46">
@@ -2125,13 +2132,17 @@
         <v>Ben's bid is stored as "Success" although it is lower than the minimum amount</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F31" s="49">
         <v>43761</v>
       </c>
-      <c r="G31" s="49"/>
-      <c r="H31" s="50"/>
+      <c r="G31" s="49">
+        <v>43763</v>
+      </c>
+      <c r="H31" s="50" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="46">
@@ -2140,18 +2151,26 @@
       <c r="B32" s="46">
         <v>3</v>
       </c>
-      <c r="C32" s="46">
+      <c r="C32" s="46" t="str">
         <f>'Bug Metrics'!$C32</f>
-        <v>0</v>
-      </c>
-      <c r="D32" s="57">
+        <v>Add Bid</v>
+      </c>
+      <c r="D32" s="57" t="str">
         <f>'Bug Metrics'!$D32</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="57"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="50"/>
+        <v>Error displayed when trying to add a bid</v>
+      </c>
+      <c r="E32" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="49">
+        <v>43763</v>
+      </c>
+      <c r="G32" s="49">
+        <v>43763</v>
+      </c>
+      <c r="H32" s="50" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="46"/>
@@ -11889,17 +11908,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="containsBlanks" dxfId="0" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(E32))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11917,8 +11936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1016"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11936,7 +11955,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -11963,13 +11982,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>33</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11980,13 +11999,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="E3" s="37" t="s">
         <v>36</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>37</v>
       </c>
       <c r="F3" s="38">
         <f t="shared" ref="F3:F216" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
@@ -12009,13 +12028,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="E4" s="38" t="s">
         <v>39</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>40</v>
       </c>
       <c r="F4" s="38">
         <f t="shared" si="0"/>
@@ -12032,13 +12051,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="24" t="s">
-        <v>42</v>
-      </c>
       <c r="E5" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="38">
         <f t="shared" si="0"/>
@@ -12055,13 +12074,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="38">
         <f t="shared" si="0"/>
@@ -12078,13 +12097,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="28" t="s">
-        <v>45</v>
-      </c>
       <c r="E7" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="38">
         <f t="shared" si="0"/>
@@ -12101,13 +12120,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="39" t="s">
         <v>46</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>47</v>
       </c>
       <c r="F8" s="38">
         <f t="shared" si="0"/>
@@ -12124,13 +12143,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="30" t="s">
-        <v>49</v>
-      </c>
       <c r="E9" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="37">
         <f t="shared" si="0"/>
@@ -12153,13 +12172,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="38">
         <f t="shared" si="0"/>
@@ -12176,13 +12195,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="28" t="s">
-        <v>52</v>
-      </c>
       <c r="E11" s="38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="38">
         <f t="shared" si="0"/>
@@ -12199,13 +12218,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="8">
         <f t="shared" si="0"/>
@@ -12222,13 +12241,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="28" t="s">
-        <v>55</v>
-      </c>
       <c r="E13" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="38">
         <f t="shared" si="0"/>
@@ -12245,13 +12264,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="28" t="s">
-        <v>64</v>
-      </c>
       <c r="E14" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="41">
         <f t="shared" si="0"/>
@@ -12268,13 +12287,13 @@
         <v>2</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="41">
         <f t="shared" si="0"/>
@@ -12291,13 +12310,13 @@
         <v>2</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="40">
         <f t="shared" si="0"/>
@@ -12314,13 +12333,13 @@
         <v>2</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="41">
         <f t="shared" si="0"/>
@@ -12337,13 +12356,13 @@
         <v>2</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="40">
         <f t="shared" si="0"/>
@@ -12360,13 +12379,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="40">
         <f t="shared" si="0"/>
@@ -12383,13 +12402,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="41">
         <f t="shared" si="0"/>
@@ -12406,13 +12425,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="41">
         <f t="shared" si="0"/>
@@ -12429,13 +12448,13 @@
         <v>2</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F22" s="41">
         <f t="shared" si="0"/>
@@ -12452,13 +12471,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="43">
         <f t="shared" si="0"/>
@@ -12475,13 +12494,13 @@
         <v>2</v>
       </c>
       <c r="C24" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="28" t="s">
-        <v>68</v>
-      </c>
       <c r="E24" s="43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" s="43">
         <f t="shared" si="0"/>
@@ -12498,13 +12517,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="28" t="s">
-        <v>72</v>
-      </c>
       <c r="E25" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" s="43">
         <f t="shared" si="0"/>
@@ -12521,13 +12540,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E26" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="58">
         <f t="shared" si="0"/>
@@ -12535,7 +12554,7 @@
       </c>
       <c r="G26" s="62">
         <f>SUM(F26:F35)</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H26" s="12" t="str">
         <f xml:space="preserve"> IF(G26&lt;10,Instructions!B7,Instructions!B8)</f>
@@ -12550,13 +12569,13 @@
         <v>3</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="58">
         <f t="shared" si="0"/>
@@ -12573,13 +12592,13 @@
         <v>3</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E28" s="56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" s="38">
         <f t="shared" si="0"/>
@@ -12596,13 +12615,13 @@
         <v>3</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E29" s="56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" s="56">
         <f t="shared" si="0"/>
@@ -12619,13 +12638,13 @@
         <v>3</v>
       </c>
       <c r="C30" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="28" t="s">
-        <v>81</v>
-      </c>
       <c r="E30" s="54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F30" s="58">
         <f t="shared" si="0"/>
@@ -12642,13 +12661,13 @@
         <v>3</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" s="54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" s="58">
         <f t="shared" si="0"/>
@@ -12664,10 +12683,19 @@
       <c r="B32" s="14">
         <v>3</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="58"/>
+      <c r="C32" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="58">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="G32" s="63"/>
       <c r="H32" s="15"/>
     </row>
@@ -18663,17 +18691,17 @@
     <mergeCell ref="G9:G25"/>
   </mergeCells>
   <conditionalFormatting sqref="H44:H1048576 H1:H15 H18:H39">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40:H43">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H17">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H16)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated mainpage.php to fix low severity bug
Co-Authored-By: tayyuliang <tayyuliang@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPMProject\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588A786A-99CB-456F-A4A7-943F9C6AF164}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62297A98-A47C-4DB2-8B22-1F89BC7ECBD4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="86">
   <si>
     <t>Severity</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>LF &amp; YL</t>
+  </si>
+  <si>
+    <t>Round 2</t>
+  </si>
+  <si>
+    <t>Bid Result displays "Pending" instead of "successful / unsuccessful"</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -708,6 +714,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1237,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1255,16 +1264,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
@@ -2090,7 +2099,7 @@
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="46">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="46">
         <v>3</v>
@@ -2099,7 +2108,7 @@
         <f>'Bug Metrics'!$C30</f>
         <v>View Bidding Results</v>
       </c>
-      <c r="D30" s="57" t="str">
+      <c r="D30" s="59" t="str">
         <f>'Bug Metrics'!$D30</f>
         <v>Min Bid Required reflects "14" although the user bidded for 12 and succeeded</v>
       </c>
@@ -2118,7 +2127,7 @@
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="46">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" s="46">
         <v>3</v>
@@ -2127,7 +2136,7 @@
         <f>'Bug Metrics'!$C31</f>
         <v>Rounds Clearing</v>
       </c>
-      <c r="D31" s="57" t="str">
+      <c r="D31" s="59" t="str">
         <f>'Bug Metrics'!$D31</f>
         <v>Ben's bid is stored as "Success" although it is lower than the minimum amount</v>
       </c>
@@ -2146,7 +2155,7 @@
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="46">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B32" s="46">
         <v>3</v>
@@ -2155,7 +2164,7 @@
         <f>'Bug Metrics'!$C32</f>
         <v>Add Bid</v>
       </c>
-      <c r="D32" s="57" t="str">
+      <c r="D32" s="59" t="str">
         <f>'Bug Metrics'!$D32</f>
         <v>Error displayed when trying to add a bid</v>
       </c>
@@ -2173,20 +2182,32 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="46"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46">
-        <f>'Bug Metrics'!$C43</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="34">
-        <f>'Bug Metrics'!$D43</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="50"/>
+      <c r="A33" s="46">
+        <v>27</v>
+      </c>
+      <c r="B33" s="46">
+        <v>3</v>
+      </c>
+      <c r="C33" s="46" t="str">
+        <f>'Bug Metrics'!$C33</f>
+        <v>Round 2</v>
+      </c>
+      <c r="D33" s="59" t="str">
+        <f>'Bug Metrics'!$D33</f>
+        <v>Bid Result displays "Pending" instead of "successful / unsuccessful"</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="49">
+        <v>43763</v>
+      </c>
+      <c r="G33" s="49">
+        <v>43763</v>
+      </c>
+      <c r="H33" s="50" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="46"/>
@@ -11937,7 +11958,7 @@
   <dimension ref="A1:H1016"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11954,16 +11975,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12011,7 +12032,7 @@
         <f t="shared" ref="F3:F216" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G3" s="62">
+      <c r="G3" s="63">
         <f>SUM($F3:$F8)</f>
         <v>27</v>
       </c>
@@ -12040,7 +12061,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="63"/>
+      <c r="G4" s="64"/>
       <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12063,7 +12084,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="63"/>
+      <c r="G5" s="64"/>
       <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12086,7 +12107,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G6" s="63"/>
+      <c r="G6" s="64"/>
       <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12109,7 +12130,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G7" s="63"/>
+      <c r="G7" s="64"/>
       <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12132,7 +12153,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G8" s="64"/>
+      <c r="G8" s="65"/>
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12155,7 +12176,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G9" s="62">
+      <c r="G9" s="63">
         <f>SUM(F9:F25)</f>
         <v>87</v>
       </c>
@@ -12184,7 +12205,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G10" s="63"/>
+      <c r="G10" s="64"/>
       <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12207,7 +12228,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G11" s="63"/>
+      <c r="G11" s="64"/>
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12230,7 +12251,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="63"/>
+      <c r="G12" s="64"/>
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12253,7 +12274,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G13" s="63"/>
+      <c r="G13" s="64"/>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12276,7 +12297,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G14" s="63"/>
+      <c r="G14" s="64"/>
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12299,7 +12320,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G15" s="63"/>
+      <c r="G15" s="64"/>
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12322,7 +12343,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G16" s="63"/>
+      <c r="G16" s="64"/>
       <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12345,7 +12366,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G17" s="63"/>
+      <c r="G17" s="64"/>
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12368,7 +12389,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12391,7 +12412,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G19" s="63"/>
+      <c r="G19" s="64"/>
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12414,7 +12435,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G20" s="63"/>
+      <c r="G20" s="64"/>
       <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12437,7 +12458,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G21" s="63"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12460,7 +12481,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G22" s="63"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12483,7 +12504,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G23" s="63"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12506,7 +12527,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="64"/>
       <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12529,7 +12550,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G25" s="63"/>
+      <c r="G25" s="64"/>
       <c r="H25" s="15"/>
     </row>
     <row r="26" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12552,9 +12573,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G26" s="62">
+      <c r="G26" s="63">
         <f>SUM(F26:F35)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H26" s="12" t="str">
         <f xml:space="preserve"> IF(G26&lt;10,Instructions!B7,Instructions!B8)</f>
@@ -12581,7 +12602,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G27" s="63"/>
+      <c r="G27" s="64"/>
       <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12604,7 +12625,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G28" s="63"/>
+      <c r="G28" s="64"/>
       <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12627,7 +12648,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G29" s="63"/>
+      <c r="G29" s="64"/>
       <c r="H29" s="15"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12650,7 +12671,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G30" s="63"/>
+      <c r="G30" s="64"/>
       <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -12673,7 +12694,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G31" s="63"/>
+      <c r="G31" s="64"/>
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12696,7 +12717,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G32" s="63"/>
+      <c r="G32" s="64"/>
       <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12706,11 +12727,20 @@
       <c r="B33" s="14">
         <v>3</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="63"/>
+      <c r="C33" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G33" s="64"/>
       <c r="H33" s="15"/>
     </row>
     <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12724,7 +12754,7 @@
       <c r="D34" s="28"/>
       <c r="E34" s="54"/>
       <c r="F34" s="54"/>
-      <c r="G34" s="63"/>
+      <c r="G34" s="64"/>
       <c r="H34" s="15"/>
     </row>
     <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12741,7 +12771,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G35" s="64"/>
+      <c r="G35" s="65"/>
       <c r="H35" s="18"/>
     </row>
     <row r="36" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12758,7 +12788,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G36" s="62">
+      <c r="G36" s="63">
         <f>SUM(F36:F39)</f>
         <v>0</v>
       </c>
@@ -12781,7 +12811,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G37" s="63"/>
+      <c r="G37" s="64"/>
       <c r="H37" s="15"/>
     </row>
     <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12798,7 +12828,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G38" s="63"/>
+      <c r="G38" s="64"/>
       <c r="H38" s="15"/>
     </row>
     <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12815,7 +12845,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G39" s="64"/>
+      <c r="G39" s="65"/>
       <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12832,7 +12862,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G40" s="62">
+      <c r="G40" s="63">
         <f>SUM(F40:F43)</f>
         <v>0</v>
       </c>
@@ -12855,7 +12885,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G41" s="63"/>
+      <c r="G41" s="64"/>
       <c r="H41" s="15"/>
     </row>
     <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12872,7 +12902,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G42" s="63"/>
+      <c r="G42" s="64"/>
       <c r="H42" s="15"/>
     </row>
     <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -12889,7 +12919,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G43" s="64"/>
+      <c r="G43" s="65"/>
       <c r="H43" s="18"/>
     </row>
     <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated BM & testcases documents
Co-Authored-By: teeyong <teeyong@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPMProject\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C58684-83A1-4BCE-A9EA-2D394E81FEF7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E158E864-D6DD-474B-9BA1-C9495BB9BBFF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="89">
   <si>
     <t>Severity</t>
   </si>
@@ -297,9 +297,6 @@
   </si>
   <si>
     <t>Bids added when Round 2 is Not Started are automatically cleared as successful</t>
-  </si>
-  <si>
-    <t>Unresolved</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1262,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2270,13 +2267,17 @@
         <v>Bids added when Round 2 is Not Started are automatically cleared as successful</v>
       </c>
       <c r="E35" s="34" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="F35" s="49">
         <v>43765</v>
       </c>
-      <c r="G35" s="49"/>
-      <c r="H35" s="50"/>
+      <c r="G35" s="49">
+        <v>43766</v>
+      </c>
+      <c r="H35" s="50" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="46"/>

</xml_diff>

<commit_message>
Updated test cases & BM
Co-Authored-By: teeyong <teeyong@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lifum\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPMProject\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FB18CC-2113-420A-9821-42211EEE079F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494BA758-88C9-4C53-BE93-BBCE93A78867}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="105">
   <si>
     <t>Severity</t>
   </si>
@@ -330,9 +330,6 @@
   </si>
   <si>
     <t>Completed courses page has no UI for header</t>
-  </si>
-  <si>
-    <t>Unresolved</t>
   </si>
   <si>
     <t>Database / Bootstrap</t>
@@ -1442,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2589,13 +2586,17 @@
         <v>Edited bid by admin is only reflected after refreshing</v>
       </c>
       <c r="E40" s="53" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="F40" s="44">
         <v>43767</v>
       </c>
-      <c r="G40" s="44"/>
-      <c r="H40" s="45"/>
+      <c r="G40" s="44">
+        <v>43768</v>
+      </c>
+      <c r="H40" s="45" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="41">
@@ -2613,13 +2614,17 @@
         <v>Completed courses page has no UI for header</v>
       </c>
       <c r="E41" s="53" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="F41" s="44">
         <v>43767</v>
       </c>
-      <c r="G41" s="44"/>
-      <c r="H41" s="45"/>
+      <c r="G41" s="44">
+        <v>43768</v>
+      </c>
+      <c r="H41" s="45" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="41">
@@ -2646,7 +2651,7 @@
         <v>43767</v>
       </c>
       <c r="H42" s="45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2665,13 +2670,17 @@
         <v>Admin UI fades slightly after clicking "show all data" in AWS</v>
       </c>
       <c r="E43" s="53" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="F43" s="44">
         <v>43767</v>
       </c>
-      <c r="G43" s="44"/>
-      <c r="H43" s="45"/>
+      <c r="G43" s="44">
+        <v>43768</v>
+      </c>
+      <c r="H43" s="45" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="41">
@@ -2743,11 +2752,17 @@
         <v>When exam timetable clashes, error message says lesson timetable clashes instead</v>
       </c>
       <c r="E46" s="57" t="s">
-        <v>100</v>
-      </c>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="45"/>
+        <v>22</v>
+      </c>
+      <c r="F46" s="44">
+        <v>43767</v>
+      </c>
+      <c r="G46" s="44">
+        <v>43768</v>
+      </c>
+      <c r="H46" s="45" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="41"/>
@@ -12380,10 +12395,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H1027"/>
+  <dimension ref="A1:H925"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView topLeftCell="A90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126:XFD227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12455,7 +12470,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="33">
-        <f t="shared" ref="F3:F227" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
+        <f t="shared" ref="F3:F125" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>1</v>
       </c>
       <c r="G3" s="80">
@@ -13446,10 +13461,10 @@
         <v>4</v>
       </c>
       <c r="C44" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44" s="68" t="s">
         <v>101</v>
-      </c>
-      <c r="D44" s="68" t="s">
-        <v>102</v>
       </c>
       <c r="E44" s="69" t="s">
         <v>46</v>
@@ -13479,7 +13494,7 @@
         <v>70</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E45" s="58" t="s">
         <v>46</v>
@@ -13503,7 +13518,7 @@
         <v>70</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E46" s="58" t="s">
         <v>36</v>
@@ -13962,7 +13977,7 @@
     </row>
     <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="51">
-        <f t="shared" ref="A74:A134" si="2">ROW()-2</f>
+        <f t="shared" ref="A74:A125" si="2">ROW()-2</f>
         <v>72</v>
       </c>
       <c r="B74" s="7"/>
@@ -14792,1594 +14807,463 @@
       <c r="G125" s="8"/>
       <c r="H125" s="8"/>
     </row>
-    <row r="126" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A126" s="51">
-        <f t="shared" si="2"/>
-        <v>124</v>
-      </c>
+    <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="7"/>
       <c r="B126" s="7"/>
-      <c r="C126" s="9"/>
-      <c r="D126" s="9"/>
-      <c r="E126" s="8"/>
-      <c r="F126" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G126" s="8"/>
-      <c r="H126" s="8"/>
-    </row>
-    <row r="127" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A127" s="51">
-        <f t="shared" si="2"/>
-        <v>125</v>
-      </c>
+    </row>
+    <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="7"/>
       <c r="B127" s="7"/>
-      <c r="C127" s="9"/>
-      <c r="D127" s="9"/>
-      <c r="E127" s="8"/>
-      <c r="F127" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G127" s="8"/>
-      <c r="H127" s="8"/>
-    </row>
-    <row r="128" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A128" s="51">
-        <f t="shared" si="2"/>
-        <v>126</v>
-      </c>
+    </row>
+    <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="7"/>
       <c r="B128" s="7"/>
-      <c r="C128" s="9"/>
-      <c r="D128" s="9"/>
-      <c r="E128" s="8"/>
-      <c r="F128" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G128" s="8"/>
-      <c r="H128" s="8"/>
-    </row>
-    <row r="129" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A129" s="51">
-        <f t="shared" si="2"/>
-        <v>127</v>
-      </c>
+    </row>
+    <row r="129" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="7"/>
       <c r="B129" s="7"/>
-      <c r="C129" s="9"/>
-      <c r="D129" s="9"/>
-      <c r="E129" s="8"/>
-      <c r="F129" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G129" s="8"/>
-      <c r="H129" s="8"/>
-    </row>
-    <row r="130" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A130" s="51">
-        <f t="shared" si="2"/>
-        <v>128</v>
-      </c>
+    </row>
+    <row r="130" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="7"/>
       <c r="B130" s="7"/>
-      <c r="C130" s="9"/>
-      <c r="D130" s="9"/>
-      <c r="E130" s="8"/>
-      <c r="F130" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G130" s="8"/>
-      <c r="H130" s="8"/>
-    </row>
-    <row r="131" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A131" s="51">
-        <f t="shared" si="2"/>
-        <v>129</v>
-      </c>
+    </row>
+    <row r="131" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="7"/>
       <c r="B131" s="7"/>
-      <c r="C131" s="9"/>
-      <c r="D131" s="9"/>
-      <c r="E131" s="8"/>
-      <c r="F131" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G131" s="8"/>
-      <c r="H131" s="8"/>
-    </row>
-    <row r="132" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A132" s="51">
-        <f t="shared" si="2"/>
-        <v>130</v>
-      </c>
+    </row>
+    <row r="132" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="7"/>
       <c r="B132" s="7"/>
-      <c r="C132" s="9"/>
-      <c r="D132" s="9"/>
-      <c r="E132" s="8"/>
-      <c r="F132" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G132" s="8"/>
-      <c r="H132" s="8"/>
-    </row>
-    <row r="133" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A133" s="51">
-        <f t="shared" si="2"/>
-        <v>131</v>
-      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="7"/>
       <c r="B133" s="7"/>
-      <c r="C133" s="9"/>
-      <c r="D133" s="9"/>
-      <c r="E133" s="8"/>
-      <c r="F133" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G133" s="8"/>
-      <c r="H133" s="8"/>
-    </row>
-    <row r="134" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A134" s="51">
-        <f t="shared" si="2"/>
-        <v>132</v>
-      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="7"/>
       <c r="B134" s="7"/>
-      <c r="C134" s="9"/>
-      <c r="D134" s="9"/>
-      <c r="E134" s="8"/>
-      <c r="F134" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G134" s="8"/>
-      <c r="H134" s="8"/>
-    </row>
-    <row r="135" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A135" s="51">
-        <v>117</v>
-      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="7"/>
       <c r="B135" s="7"/>
-      <c r="C135" s="9"/>
-      <c r="D135" s="9"/>
-      <c r="E135" s="8"/>
-      <c r="F135" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G135" s="8"/>
-      <c r="H135" s="8"/>
-    </row>
-    <row r="136" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A136" s="51">
-        <v>118</v>
-      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="7"/>
       <c r="B136" s="7"/>
-      <c r="C136" s="9"/>
-      <c r="D136" s="9"/>
-      <c r="E136" s="8"/>
-      <c r="F136" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G136" s="8"/>
-      <c r="H136" s="8"/>
-    </row>
-    <row r="137" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A137" s="51">
-        <v>119</v>
-      </c>
+    </row>
+    <row r="137" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="7"/>
       <c r="B137" s="7"/>
-      <c r="C137" s="9"/>
-      <c r="D137" s="9"/>
-      <c r="E137" s="8"/>
-      <c r="F137" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G137" s="8"/>
-      <c r="H137" s="8"/>
-    </row>
-    <row r="138" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A138" s="51">
-        <v>120</v>
-      </c>
+    </row>
+    <row r="138" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="7"/>
       <c r="B138" s="7"/>
-      <c r="C138" s="9"/>
-      <c r="D138" s="9"/>
-      <c r="E138" s="8"/>
-      <c r="F138" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G138" s="8"/>
-      <c r="H138" s="8"/>
-    </row>
-    <row r="139" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A139" s="51">
-        <v>121</v>
-      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="7"/>
       <c r="B139" s="7"/>
-      <c r="C139" s="9"/>
-      <c r="D139" s="9"/>
-      <c r="E139" s="8"/>
-      <c r="F139" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G139" s="8"/>
-      <c r="H139" s="8"/>
-    </row>
-    <row r="140" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A140" s="51">
-        <v>122</v>
-      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="7"/>
       <c r="B140" s="7"/>
-      <c r="C140" s="9"/>
-      <c r="D140" s="9"/>
-      <c r="E140" s="8"/>
-      <c r="F140" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G140" s="8"/>
-      <c r="H140" s="8"/>
-    </row>
-    <row r="141" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A141" s="51">
-        <v>123</v>
-      </c>
+    </row>
+    <row r="141" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="7"/>
       <c r="B141" s="7"/>
-      <c r="C141" s="9"/>
-      <c r="D141" s="9"/>
-      <c r="E141" s="8"/>
-      <c r="F141" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G141" s="8"/>
-      <c r="H141" s="8"/>
-    </row>
-    <row r="142" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A142" s="51">
-        <v>124</v>
-      </c>
+    </row>
+    <row r="142" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="7"/>
       <c r="B142" s="7"/>
-      <c r="C142" s="9"/>
-      <c r="D142" s="9"/>
-      <c r="E142" s="8"/>
-      <c r="F142" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G142" s="8"/>
-      <c r="H142" s="8"/>
-    </row>
-    <row r="143" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A143" s="51">
-        <v>125</v>
-      </c>
+    </row>
+    <row r="143" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="7"/>
       <c r="B143" s="7"/>
-      <c r="C143" s="9"/>
-      <c r="D143" s="9"/>
-      <c r="E143" s="8"/>
-      <c r="F143" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G143" s="8"/>
-      <c r="H143" s="8"/>
-    </row>
-    <row r="144" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A144" s="51">
-        <v>126</v>
-      </c>
+    </row>
+    <row r="144" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="7"/>
       <c r="B144" s="7"/>
-      <c r="C144" s="9"/>
-      <c r="D144" s="9"/>
-      <c r="E144" s="8"/>
-      <c r="F144" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G144" s="8"/>
-      <c r="H144" s="8"/>
-    </row>
-    <row r="145" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A145" s="51">
-        <v>127</v>
-      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="7"/>
       <c r="B145" s="7"/>
-      <c r="C145" s="9"/>
-      <c r="D145" s="9"/>
-      <c r="E145" s="8"/>
-      <c r="F145" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G145" s="8"/>
-      <c r="H145" s="8"/>
-    </row>
-    <row r="146" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A146" s="51">
-        <v>128</v>
-      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="7"/>
       <c r="B146" s="7"/>
-      <c r="C146" s="9"/>
-      <c r="D146" s="9"/>
-      <c r="E146" s="8"/>
-      <c r="F146" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G146" s="8"/>
-      <c r="H146" s="8"/>
-    </row>
-    <row r="147" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A147" s="51">
-        <v>129</v>
-      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="7"/>
       <c r="B147" s="7"/>
-      <c r="C147" s="9"/>
-      <c r="D147" s="9"/>
-      <c r="E147" s="8"/>
-      <c r="F147" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G147" s="8"/>
-      <c r="H147" s="8"/>
-    </row>
-    <row r="148" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A148" s="51">
-        <v>130</v>
-      </c>
+    </row>
+    <row r="148" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="7"/>
       <c r="B148" s="7"/>
-      <c r="C148" s="9"/>
-      <c r="D148" s="9"/>
-      <c r="E148" s="8"/>
-      <c r="F148" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G148" s="8"/>
-      <c r="H148" s="8"/>
-    </row>
-    <row r="149" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A149" s="51">
-        <v>131</v>
-      </c>
+    </row>
+    <row r="149" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="7"/>
       <c r="B149" s="7"/>
-      <c r="C149" s="9"/>
-      <c r="D149" s="9"/>
-      <c r="E149" s="8"/>
-      <c r="F149" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G149" s="8"/>
-      <c r="H149" s="8"/>
-    </row>
-    <row r="150" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A150" s="51">
-        <v>132</v>
-      </c>
+    </row>
+    <row r="150" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="7"/>
       <c r="B150" s="7"/>
-      <c r="C150" s="9"/>
-      <c r="D150" s="9"/>
-      <c r="E150" s="8"/>
-      <c r="F150" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G150" s="8"/>
-      <c r="H150" s="8"/>
-    </row>
-    <row r="151" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A151" s="51">
-        <v>133</v>
-      </c>
+    </row>
+    <row r="151" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="7"/>
       <c r="B151" s="7"/>
-      <c r="C151" s="9"/>
-      <c r="D151" s="9"/>
-      <c r="E151" s="8"/>
-      <c r="F151" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G151" s="8"/>
-      <c r="H151" s="8"/>
-    </row>
-    <row r="152" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A152" s="51">
-        <v>134</v>
-      </c>
+    </row>
+    <row r="152" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="7"/>
       <c r="B152" s="7"/>
-      <c r="C152" s="9"/>
-      <c r="D152" s="9"/>
-      <c r="E152" s="8"/>
-      <c r="F152" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G152" s="8"/>
-      <c r="H152" s="8"/>
-    </row>
-    <row r="153" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A153" s="51">
-        <v>135</v>
-      </c>
+    </row>
+    <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="7"/>
       <c r="B153" s="7"/>
-      <c r="C153" s="9"/>
-      <c r="D153" s="9"/>
-      <c r="E153" s="8"/>
-      <c r="F153" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G153" s="8"/>
-      <c r="H153" s="8"/>
-    </row>
-    <row r="154" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A154" s="51">
-        <v>136</v>
-      </c>
+    </row>
+    <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="7"/>
       <c r="B154" s="7"/>
-      <c r="C154" s="9"/>
-      <c r="D154" s="9"/>
-      <c r="E154" s="8"/>
-      <c r="F154" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G154" s="8"/>
-      <c r="H154" s="8"/>
-    </row>
-    <row r="155" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A155" s="51">
-        <v>137</v>
-      </c>
+    </row>
+    <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="7"/>
       <c r="B155" s="7"/>
-      <c r="C155" s="9"/>
-      <c r="D155" s="9"/>
-      <c r="E155" s="8"/>
-      <c r="F155" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G155" s="8"/>
-      <c r="H155" s="8"/>
-    </row>
-    <row r="156" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A156" s="51">
-        <v>138</v>
-      </c>
+    </row>
+    <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="7"/>
       <c r="B156" s="7"/>
-      <c r="C156" s="9"/>
-      <c r="D156" s="9"/>
-      <c r="E156" s="8"/>
-      <c r="F156" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G156" s="8"/>
-      <c r="H156" s="8"/>
-    </row>
-    <row r="157" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A157" s="51">
-        <v>139</v>
-      </c>
+    </row>
+    <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="7"/>
       <c r="B157" s="7"/>
-      <c r="C157" s="9"/>
-      <c r="D157" s="9"/>
-      <c r="E157" s="8"/>
-      <c r="F157" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G157" s="8"/>
-      <c r="H157" s="8"/>
-    </row>
-    <row r="158" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A158" s="51">
-        <v>140</v>
-      </c>
+    </row>
+    <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="7"/>
       <c r="B158" s="7"/>
-      <c r="C158" s="9"/>
-      <c r="D158" s="9"/>
-      <c r="E158" s="8"/>
-      <c r="F158" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G158" s="8"/>
-      <c r="H158" s="8"/>
-    </row>
-    <row r="159" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A159" s="51">
-        <v>141</v>
-      </c>
+    </row>
+    <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="7"/>
       <c r="B159" s="7"/>
-      <c r="C159" s="9"/>
-      <c r="D159" s="9"/>
-      <c r="E159" s="8"/>
-      <c r="F159" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G159" s="8"/>
-      <c r="H159" s="8"/>
-    </row>
-    <row r="160" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A160" s="51">
-        <v>142</v>
-      </c>
+    </row>
+    <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="7"/>
       <c r="B160" s="7"/>
-      <c r="C160" s="9"/>
-      <c r="D160" s="9"/>
-      <c r="E160" s="8"/>
-      <c r="F160" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G160" s="8"/>
-      <c r="H160" s="8"/>
-    </row>
-    <row r="161" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A161" s="51">
-        <v>143</v>
-      </c>
+    </row>
+    <row r="161" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="7"/>
       <c r="B161" s="7"/>
-      <c r="C161" s="9"/>
-      <c r="D161" s="9"/>
-      <c r="E161" s="8"/>
-      <c r="F161" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G161" s="8"/>
-      <c r="H161" s="8"/>
-    </row>
-    <row r="162" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A162" s="51">
-        <v>144</v>
-      </c>
+    </row>
+    <row r="162" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="7"/>
       <c r="B162" s="7"/>
-      <c r="C162" s="9"/>
-      <c r="D162" s="9"/>
-      <c r="E162" s="8"/>
-      <c r="F162" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G162" s="8"/>
-      <c r="H162" s="8"/>
-    </row>
-    <row r="163" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A163" s="51">
-        <v>145</v>
-      </c>
+    </row>
+    <row r="163" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="7"/>
       <c r="B163" s="7"/>
-      <c r="C163" s="9"/>
-      <c r="D163" s="9"/>
-      <c r="E163" s="8"/>
-      <c r="F163" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G163" s="8"/>
-      <c r="H163" s="8"/>
-    </row>
-    <row r="164" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A164" s="51">
-        <v>146</v>
-      </c>
+    </row>
+    <row r="164" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="7"/>
       <c r="B164" s="7"/>
-      <c r="C164" s="9"/>
-      <c r="D164" s="9"/>
-      <c r="E164" s="8"/>
-      <c r="F164" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G164" s="8"/>
-      <c r="H164" s="8"/>
-    </row>
-    <row r="165" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A165" s="51">
-        <v>147</v>
-      </c>
+    </row>
+    <row r="165" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="7"/>
       <c r="B165" s="7"/>
-      <c r="C165" s="9"/>
-      <c r="D165" s="9"/>
-      <c r="E165" s="8"/>
-      <c r="F165" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G165" s="8"/>
-      <c r="H165" s="8"/>
-    </row>
-    <row r="166" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A166" s="51">
-        <v>148</v>
-      </c>
+    </row>
+    <row r="166" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="7"/>
       <c r="B166" s="7"/>
-      <c r="C166" s="9"/>
-      <c r="D166" s="9"/>
-      <c r="E166" s="8"/>
-      <c r="F166" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G166" s="8"/>
-      <c r="H166" s="8"/>
-    </row>
-    <row r="167" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A167" s="51">
-        <v>149</v>
-      </c>
+    </row>
+    <row r="167" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="7"/>
       <c r="B167" s="7"/>
-      <c r="C167" s="9"/>
-      <c r="D167" s="9"/>
-      <c r="E167" s="8"/>
-      <c r="F167" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G167" s="8"/>
-      <c r="H167" s="8"/>
-    </row>
-    <row r="168" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A168" s="51">
-        <v>150</v>
-      </c>
+    </row>
+    <row r="168" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="7"/>
       <c r="B168" s="7"/>
-      <c r="C168" s="9"/>
-      <c r="D168" s="9"/>
-      <c r="E168" s="8"/>
-      <c r="F168" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G168" s="8"/>
-      <c r="H168" s="8"/>
-    </row>
-    <row r="169" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A169" s="51">
-        <v>151</v>
-      </c>
+    </row>
+    <row r="169" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="7"/>
       <c r="B169" s="7"/>
-      <c r="C169" s="9"/>
-      <c r="D169" s="9"/>
-      <c r="E169" s="8"/>
-      <c r="F169" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G169" s="8"/>
-      <c r="H169" s="8"/>
-    </row>
-    <row r="170" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A170" s="51">
-        <v>152</v>
-      </c>
+    </row>
+    <row r="170" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="7"/>
       <c r="B170" s="7"/>
-      <c r="C170" s="9"/>
-      <c r="D170" s="9"/>
-      <c r="E170" s="8"/>
-      <c r="F170" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G170" s="8"/>
-      <c r="H170" s="8"/>
-    </row>
-    <row r="171" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A171" s="51">
-        <v>153</v>
-      </c>
+    </row>
+    <row r="171" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="7"/>
       <c r="B171" s="7"/>
-      <c r="C171" s="9"/>
-      <c r="D171" s="9"/>
-      <c r="E171" s="8"/>
-      <c r="F171" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G171" s="8"/>
-      <c r="H171" s="8"/>
-    </row>
-    <row r="172" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A172" s="51">
-        <v>154</v>
-      </c>
+    </row>
+    <row r="172" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="7"/>
       <c r="B172" s="7"/>
-      <c r="C172" s="9"/>
-      <c r="D172" s="9"/>
-      <c r="E172" s="8"/>
-      <c r="F172" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G172" s="8"/>
-      <c r="H172" s="8"/>
-    </row>
-    <row r="173" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A173" s="51">
-        <v>155</v>
-      </c>
+    </row>
+    <row r="173" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="7"/>
       <c r="B173" s="7"/>
-      <c r="C173" s="9"/>
-      <c r="D173" s="9"/>
-      <c r="E173" s="8"/>
-      <c r="F173" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G173" s="8"/>
-      <c r="H173" s="8"/>
-    </row>
-    <row r="174" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A174" s="51">
-        <v>156</v>
-      </c>
+    </row>
+    <row r="174" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="7"/>
       <c r="B174" s="7"/>
-      <c r="C174" s="9"/>
-      <c r="D174" s="9"/>
-      <c r="E174" s="8"/>
-      <c r="F174" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G174" s="8"/>
-      <c r="H174" s="8"/>
-    </row>
-    <row r="175" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A175" s="51">
-        <v>157</v>
-      </c>
+    </row>
+    <row r="175" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="7"/>
       <c r="B175" s="7"/>
-      <c r="C175" s="9"/>
-      <c r="D175" s="9"/>
-      <c r="E175" s="8"/>
-      <c r="F175" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G175" s="8"/>
-      <c r="H175" s="8"/>
-    </row>
-    <row r="176" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A176" s="51">
-        <v>158</v>
-      </c>
+    </row>
+    <row r="176" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="7"/>
       <c r="B176" s="7"/>
-      <c r="C176" s="9"/>
-      <c r="D176" s="9"/>
-      <c r="E176" s="8"/>
-      <c r="F176" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G176" s="8"/>
-      <c r="H176" s="8"/>
-    </row>
-    <row r="177" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A177" s="51">
-        <v>159</v>
-      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="7"/>
       <c r="B177" s="7"/>
-      <c r="C177" s="9"/>
-      <c r="D177" s="9"/>
-      <c r="E177" s="8"/>
-      <c r="F177" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G177" s="8"/>
-      <c r="H177" s="8"/>
-    </row>
-    <row r="178" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A178" s="51">
-        <v>160</v>
-      </c>
+    </row>
+    <row r="178" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="7"/>
       <c r="B178" s="7"/>
-      <c r="C178" s="9"/>
-      <c r="D178" s="9"/>
-      <c r="E178" s="8"/>
-      <c r="F178" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G178" s="8"/>
-      <c r="H178" s="8"/>
-    </row>
-    <row r="179" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A179" s="51">
-        <v>161</v>
-      </c>
+    </row>
+    <row r="179" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="7"/>
       <c r="B179" s="7"/>
-      <c r="C179" s="9"/>
-      <c r="D179" s="9"/>
-      <c r="E179" s="8"/>
-      <c r="F179" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G179" s="8"/>
-      <c r="H179" s="8"/>
-    </row>
-    <row r="180" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A180" s="51">
-        <v>162</v>
-      </c>
+    </row>
+    <row r="180" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="7"/>
       <c r="B180" s="7"/>
-      <c r="C180" s="9"/>
-      <c r="D180" s="9"/>
-      <c r="E180" s="8"/>
-      <c r="F180" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G180" s="8"/>
-      <c r="H180" s="8"/>
-    </row>
-    <row r="181" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A181" s="51">
-        <v>163</v>
-      </c>
+    </row>
+    <row r="181" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="7"/>
       <c r="B181" s="7"/>
-      <c r="C181" s="9"/>
-      <c r="D181" s="9"/>
-      <c r="E181" s="8"/>
-      <c r="F181" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G181" s="8"/>
-      <c r="H181" s="8"/>
-    </row>
-    <row r="182" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A182" s="51">
-        <v>164</v>
-      </c>
+    </row>
+    <row r="182" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="7"/>
       <c r="B182" s="7"/>
-      <c r="C182" s="9"/>
-      <c r="D182" s="9"/>
-      <c r="E182" s="8"/>
-      <c r="F182" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G182" s="8"/>
-      <c r="H182" s="8"/>
-    </row>
-    <row r="183" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A183" s="51">
-        <v>165</v>
-      </c>
+    </row>
+    <row r="183" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="7"/>
       <c r="B183" s="7"/>
-      <c r="C183" s="9"/>
-      <c r="D183" s="9"/>
-      <c r="E183" s="8"/>
-      <c r="F183" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G183" s="8"/>
-      <c r="H183" s="8"/>
-    </row>
-    <row r="184" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A184" s="51">
-        <v>166</v>
-      </c>
+    </row>
+    <row r="184" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="7"/>
       <c r="B184" s="7"/>
-      <c r="C184" s="9"/>
-      <c r="D184" s="9"/>
-      <c r="E184" s="8"/>
-      <c r="F184" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G184" s="8"/>
-      <c r="H184" s="8"/>
-    </row>
-    <row r="185" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A185" s="51">
-        <v>167</v>
-      </c>
+    </row>
+    <row r="185" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="7"/>
       <c r="B185" s="7"/>
-      <c r="C185" s="9"/>
-      <c r="D185" s="9"/>
-      <c r="E185" s="8"/>
-      <c r="F185" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G185" s="8"/>
-      <c r="H185" s="8"/>
-    </row>
-    <row r="186" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A186" s="51">
-        <v>168</v>
-      </c>
+    </row>
+    <row r="186" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="7"/>
       <c r="B186" s="7"/>
-      <c r="C186" s="9"/>
-      <c r="D186" s="9"/>
-      <c r="E186" s="8"/>
-      <c r="F186" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G186" s="8"/>
-      <c r="H186" s="8"/>
-    </row>
-    <row r="187" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A187" s="51">
-        <v>169</v>
-      </c>
+    </row>
+    <row r="187" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="7"/>
       <c r="B187" s="7"/>
-      <c r="C187" s="9"/>
-      <c r="D187" s="9"/>
-      <c r="E187" s="8"/>
-      <c r="F187" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G187" s="8"/>
-      <c r="H187" s="8"/>
-    </row>
-    <row r="188" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A188" s="51">
-        <v>170</v>
-      </c>
+    </row>
+    <row r="188" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="7"/>
       <c r="B188" s="7"/>
-      <c r="C188" s="9"/>
-      <c r="D188" s="9"/>
-      <c r="E188" s="8"/>
-      <c r="F188" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G188" s="8"/>
-      <c r="H188" s="8"/>
-    </row>
-    <row r="189" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A189" s="51">
-        <v>171</v>
-      </c>
+    </row>
+    <row r="189" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="7"/>
       <c r="B189" s="7"/>
-      <c r="C189" s="9"/>
-      <c r="D189" s="9"/>
-      <c r="E189" s="8"/>
-      <c r="F189" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G189" s="8"/>
-      <c r="H189" s="8"/>
-    </row>
-    <row r="190" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A190" s="51">
-        <v>172</v>
-      </c>
+    </row>
+    <row r="190" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="7"/>
       <c r="B190" s="7"/>
-      <c r="C190" s="9"/>
-      <c r="D190" s="9"/>
-      <c r="E190" s="8"/>
-      <c r="F190" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G190" s="8"/>
-      <c r="H190" s="8"/>
-    </row>
-    <row r="191" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A191" s="51">
-        <v>173</v>
-      </c>
+    </row>
+    <row r="191" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="7"/>
       <c r="B191" s="7"/>
-      <c r="C191" s="9"/>
-      <c r="D191" s="9"/>
-      <c r="E191" s="8"/>
-      <c r="F191" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G191" s="8"/>
-      <c r="H191" s="8"/>
-    </row>
-    <row r="192" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A192" s="51">
-        <v>174</v>
-      </c>
+    </row>
+    <row r="192" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="7"/>
       <c r="B192" s="7"/>
-      <c r="C192" s="9"/>
-      <c r="D192" s="9"/>
-      <c r="E192" s="8"/>
-      <c r="F192" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G192" s="8"/>
-      <c r="H192" s="8"/>
-    </row>
-    <row r="193" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A193" s="51">
-        <v>175</v>
-      </c>
+    </row>
+    <row r="193" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="7"/>
       <c r="B193" s="7"/>
-      <c r="C193" s="9"/>
-      <c r="D193" s="9"/>
-      <c r="E193" s="8"/>
-      <c r="F193" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G193" s="8"/>
-      <c r="H193" s="8"/>
-    </row>
-    <row r="194" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A194" s="51">
-        <v>176</v>
-      </c>
+    </row>
+    <row r="194" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="7"/>
       <c r="B194" s="7"/>
-      <c r="C194" s="9"/>
-      <c r="D194" s="9"/>
-      <c r="E194" s="8"/>
-      <c r="F194" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G194" s="8"/>
-      <c r="H194" s="8"/>
-    </row>
-    <row r="195" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A195" s="51">
-        <v>177</v>
-      </c>
+    </row>
+    <row r="195" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="7"/>
       <c r="B195" s="7"/>
-      <c r="C195" s="9"/>
-      <c r="D195" s="9"/>
-      <c r="E195" s="8"/>
-      <c r="F195" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G195" s="8"/>
-      <c r="H195" s="8"/>
-    </row>
-    <row r="196" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A196" s="51">
-        <v>178</v>
-      </c>
+    </row>
+    <row r="196" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="7"/>
       <c r="B196" s="7"/>
-      <c r="C196" s="9"/>
-      <c r="D196" s="9"/>
-      <c r="E196" s="8"/>
-      <c r="F196" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G196" s="8"/>
-      <c r="H196" s="8"/>
-    </row>
-    <row r="197" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A197" s="51">
-        <v>168</v>
-      </c>
+    </row>
+    <row r="197" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="7"/>
       <c r="B197" s="7"/>
-      <c r="C197" s="9"/>
-      <c r="D197" s="9"/>
-      <c r="E197" s="8"/>
-      <c r="F197" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G197" s="8"/>
-      <c r="H197" s="8"/>
-    </row>
-    <row r="198" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A198" s="51">
-        <v>169</v>
-      </c>
+    </row>
+    <row r="198" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="7"/>
       <c r="B198" s="7"/>
-      <c r="C198" s="9"/>
-      <c r="D198" s="9"/>
-      <c r="E198" s="8"/>
-      <c r="F198" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G198" s="8"/>
-      <c r="H198" s="8"/>
-    </row>
-    <row r="199" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A199" s="51">
-        <v>170</v>
-      </c>
+    </row>
+    <row r="199" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="7"/>
       <c r="B199" s="7"/>
-      <c r="C199" s="9"/>
-      <c r="D199" s="9"/>
-      <c r="E199" s="8"/>
-      <c r="F199" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G199" s="8"/>
-      <c r="H199" s="8"/>
-    </row>
-    <row r="200" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A200" s="51">
-        <v>171</v>
-      </c>
+    </row>
+    <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="7"/>
       <c r="B200" s="7"/>
-      <c r="C200" s="9"/>
-      <c r="D200" s="9"/>
-      <c r="E200" s="8"/>
-      <c r="F200" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G200" s="8"/>
-      <c r="H200" s="8"/>
-    </row>
-    <row r="201" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A201" s="51">
-        <v>172</v>
-      </c>
+    </row>
+    <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="7"/>
       <c r="B201" s="7"/>
-      <c r="C201" s="9"/>
-      <c r="D201" s="9"/>
-      <c r="E201" s="8"/>
-      <c r="F201" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G201" s="8"/>
-      <c r="H201" s="8"/>
-    </row>
-    <row r="202" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A202" s="51">
-        <v>173</v>
-      </c>
+    </row>
+    <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="7"/>
       <c r="B202" s="7"/>
-      <c r="C202" s="9"/>
-      <c r="D202" s="9"/>
-      <c r="E202" s="8"/>
-      <c r="F202" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G202" s="8"/>
-      <c r="H202" s="8"/>
-    </row>
-    <row r="203" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A203" s="51">
-        <v>174</v>
-      </c>
+    </row>
+    <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="7"/>
       <c r="B203" s="7"/>
-      <c r="C203" s="9"/>
-      <c r="D203" s="9"/>
-      <c r="E203" s="8"/>
-      <c r="F203" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G203" s="8"/>
-      <c r="H203" s="8"/>
-    </row>
-    <row r="204" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A204" s="51">
-        <v>175</v>
-      </c>
+    </row>
+    <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="7"/>
       <c r="B204" s="7"/>
-      <c r="C204" s="9"/>
-      <c r="D204" s="9"/>
-      <c r="E204" s="8"/>
-      <c r="F204" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G204" s="8"/>
-      <c r="H204" s="8"/>
-    </row>
-    <row r="205" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A205" s="51">
-        <v>176</v>
-      </c>
+    </row>
+    <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="7"/>
       <c r="B205" s="7"/>
-      <c r="C205" s="9"/>
-      <c r="D205" s="9"/>
-      <c r="E205" s="8"/>
-      <c r="F205" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G205" s="8"/>
-      <c r="H205" s="8"/>
-    </row>
-    <row r="206" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A206" s="51">
-        <v>177</v>
-      </c>
+    </row>
+    <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="7"/>
       <c r="B206" s="7"/>
-      <c r="C206" s="9"/>
-      <c r="D206" s="9"/>
-      <c r="E206" s="8"/>
-      <c r="F206" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G206" s="8"/>
-      <c r="H206" s="8"/>
-    </row>
-    <row r="207" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A207" s="51">
-        <v>178</v>
-      </c>
+    </row>
+    <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="7"/>
       <c r="B207" s="7"/>
-      <c r="C207" s="9"/>
-      <c r="D207" s="9"/>
-      <c r="E207" s="8"/>
-      <c r="F207" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G207" s="8"/>
-      <c r="H207" s="8"/>
-    </row>
-    <row r="208" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A208" s="51">
-        <v>179</v>
-      </c>
+    </row>
+    <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="7"/>
       <c r="B208" s="7"/>
-      <c r="C208" s="9"/>
-      <c r="D208" s="9"/>
-      <c r="E208" s="8"/>
-      <c r="F208" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G208" s="8"/>
-      <c r="H208" s="8"/>
-    </row>
-    <row r="209" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A209" s="51">
-        <v>180</v>
-      </c>
+    </row>
+    <row r="209" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="7"/>
       <c r="B209" s="7"/>
-      <c r="C209" s="9"/>
-      <c r="D209" s="9"/>
-      <c r="E209" s="8"/>
-      <c r="F209" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G209" s="8"/>
-      <c r="H209" s="8"/>
-    </row>
-    <row r="210" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A210" s="51">
-        <v>181</v>
-      </c>
+    </row>
+    <row r="210" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="7"/>
       <c r="B210" s="7"/>
-      <c r="C210" s="9"/>
-      <c r="D210" s="9"/>
-      <c r="E210" s="8"/>
-      <c r="F210" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G210" s="8"/>
-      <c r="H210" s="8"/>
-    </row>
-    <row r="211" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A211" s="51">
-        <v>182</v>
-      </c>
+    </row>
+    <row r="211" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="7"/>
       <c r="B211" s="7"/>
-      <c r="C211" s="9"/>
-      <c r="D211" s="9"/>
-      <c r="E211" s="8"/>
-      <c r="F211" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G211" s="8"/>
-      <c r="H211" s="8"/>
-    </row>
-    <row r="212" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A212" s="51">
-        <v>183</v>
-      </c>
+    </row>
+    <row r="212" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="7"/>
       <c r="B212" s="7"/>
-      <c r="C212" s="9"/>
-      <c r="D212" s="9"/>
-      <c r="E212" s="8"/>
-      <c r="F212" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G212" s="8"/>
-      <c r="H212" s="8"/>
-    </row>
-    <row r="213" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A213" s="8">
-        <v>184</v>
-      </c>
+    </row>
+    <row r="213" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="7"/>
       <c r="B213" s="7"/>
-      <c r="C213" s="9"/>
-      <c r="D213" s="9"/>
-      <c r="E213" s="8"/>
-      <c r="F213" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G213" s="8"/>
-      <c r="H213" s="8"/>
-    </row>
-    <row r="214" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A214" s="8">
-        <v>185</v>
-      </c>
+    </row>
+    <row r="214" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="7"/>
       <c r="B214" s="7"/>
-      <c r="C214" s="9"/>
-      <c r="D214" s="9"/>
-      <c r="E214" s="8"/>
-      <c r="F214" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G214" s="8"/>
-      <c r="H214" s="8"/>
-    </row>
-    <row r="215" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A215" s="8">
-        <v>186</v>
-      </c>
+    </row>
+    <row r="215" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="7"/>
       <c r="B215" s="7"/>
-      <c r="C215" s="9"/>
-      <c r="D215" s="9"/>
-      <c r="E215" s="8"/>
-      <c r="F215" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G215" s="8"/>
-      <c r="H215" s="8"/>
-    </row>
-    <row r="216" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A216" s="8">
-        <v>187</v>
-      </c>
+    </row>
+    <row r="216" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="7"/>
       <c r="B216" s="7"/>
-      <c r="C216" s="9"/>
-      <c r="D216" s="9"/>
-      <c r="E216" s="8"/>
-      <c r="F216" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G216" s="8"/>
-      <c r="H216" s="8"/>
-    </row>
-    <row r="217" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A217" s="8">
-        <v>188</v>
-      </c>
+    </row>
+    <row r="217" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="7"/>
       <c r="B217" s="7"/>
-      <c r="C217" s="9"/>
-      <c r="D217" s="9"/>
-      <c r="E217" s="8"/>
-      <c r="F217" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G217" s="8"/>
-      <c r="H217" s="8"/>
-    </row>
-    <row r="218" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A218" s="8">
-        <v>189</v>
-      </c>
+    </row>
+    <row r="218" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="7"/>
       <c r="B218" s="7"/>
-      <c r="C218" s="9"/>
-      <c r="D218" s="9"/>
-      <c r="E218" s="8"/>
-      <c r="F218" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G218" s="8"/>
-      <c r="H218" s="8"/>
-    </row>
-    <row r="219" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A219" s="8">
-        <v>190</v>
-      </c>
+    </row>
+    <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="7"/>
       <c r="B219" s="7"/>
-      <c r="C219" s="9"/>
-      <c r="D219" s="9"/>
-      <c r="E219" s="8"/>
-      <c r="F219" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G219" s="8"/>
-      <c r="H219" s="8"/>
-    </row>
-    <row r="220" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A220" s="8">
-        <v>191</v>
-      </c>
+    </row>
+    <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A220" s="7"/>
       <c r="B220" s="7"/>
-      <c r="C220" s="9"/>
-      <c r="D220" s="9"/>
-      <c r="E220" s="8"/>
-      <c r="F220" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G220" s="8"/>
-      <c r="H220" s="8"/>
-    </row>
-    <row r="221" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A221" s="8">
-        <v>192</v>
-      </c>
+    </row>
+    <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="7"/>
       <c r="B221" s="7"/>
-      <c r="C221" s="9"/>
-      <c r="D221" s="9"/>
-      <c r="E221" s="8"/>
-      <c r="F221" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G221" s="8"/>
-      <c r="H221" s="8"/>
-    </row>
-    <row r="222" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A222" s="8">
-        <v>193</v>
-      </c>
+    </row>
+    <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A222" s="7"/>
       <c r="B222" s="7"/>
-      <c r="C222" s="9"/>
-      <c r="D222" s="9"/>
-      <c r="E222" s="8"/>
-      <c r="F222" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G222" s="8"/>
-      <c r="H222" s="8"/>
-    </row>
-    <row r="223" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A223" s="8">
-        <v>194</v>
-      </c>
+    </row>
+    <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A223" s="7"/>
       <c r="B223" s="7"/>
-      <c r="C223" s="9"/>
-      <c r="D223" s="9"/>
-      <c r="E223" s="8"/>
-      <c r="F223" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G223" s="8"/>
-      <c r="H223" s="8"/>
-    </row>
-    <row r="224" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A224" s="8">
-        <v>195</v>
-      </c>
+    </row>
+    <row r="224" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A224" s="7"/>
       <c r="B224" s="7"/>
-      <c r="C224" s="9"/>
-      <c r="D224" s="9"/>
-      <c r="E224" s="8"/>
-      <c r="F224" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G224" s="8"/>
-      <c r="H224" s="8"/>
-    </row>
-    <row r="225" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A225" s="8">
-        <v>196</v>
-      </c>
+    </row>
+    <row r="225" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="7"/>
       <c r="B225" s="7"/>
-      <c r="C225" s="9"/>
-      <c r="D225" s="9"/>
-      <c r="E225" s="8"/>
-      <c r="F225" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G225" s="8"/>
-      <c r="H225" s="8"/>
-    </row>
-    <row r="226" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A226" s="8">
-        <v>197</v>
-      </c>
+    </row>
+    <row r="226" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="7"/>
       <c r="B226" s="7"/>
-      <c r="C226" s="9"/>
-      <c r="D226" s="9"/>
-      <c r="E226" s="8"/>
-      <c r="F226" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G226" s="8"/>
-      <c r="H226" s="8"/>
-    </row>
-    <row r="227" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A227" s="8">
-        <v>198</v>
-      </c>
+    </row>
+    <row r="227" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="7"/>
       <c r="B227" s="7"/>
-      <c r="C227" s="9"/>
-      <c r="D227" s="9"/>
-      <c r="E227" s="8"/>
-      <c r="F227" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G227" s="8"/>
-      <c r="H227" s="8"/>
-    </row>
-    <row r="228" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="228" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="7"/>
       <c r="B228" s="7"/>
     </row>
-    <row r="229" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="7"/>
       <c r="B229" s="7"/>
     </row>
-    <row r="230" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="7"/>
       <c r="B230" s="7"/>
     </row>
-    <row r="231" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="7"/>
       <c r="B231" s="7"/>
     </row>
-    <row r="232" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="7"/>
       <c r="B232" s="7"/>
     </row>
-    <row r="233" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="7"/>
       <c r="B233" s="7"/>
     </row>
-    <row r="234" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="7"/>
       <c r="B234" s="7"/>
     </row>
-    <row r="235" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="7"/>
       <c r="B235" s="7"/>
     </row>
-    <row r="236" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="7"/>
       <c r="B236" s="7"/>
     </row>
-    <row r="237" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="7"/>
       <c r="B237" s="7"/>
     </row>
-    <row r="238" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="7"/>
       <c r="B238" s="7"/>
     </row>
-    <row r="239" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="7"/>
       <c r="B239" s="7"/>
     </row>
-    <row r="240" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="7"/>
       <c r="B240" s="7"/>
     </row>
@@ -19122,414 +18006,6 @@
     <row r="925" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A925" s="7"/>
       <c r="B925" s="7"/>
-    </row>
-    <row r="926" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A926" s="7"/>
-      <c r="B926" s="7"/>
-    </row>
-    <row r="927" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A927" s="7"/>
-      <c r="B927" s="7"/>
-    </row>
-    <row r="928" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A928" s="7"/>
-      <c r="B928" s="7"/>
-    </row>
-    <row r="929" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A929" s="7"/>
-      <c r="B929" s="7"/>
-    </row>
-    <row r="930" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A930" s="7"/>
-      <c r="B930" s="7"/>
-    </row>
-    <row r="931" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A931" s="7"/>
-      <c r="B931" s="7"/>
-    </row>
-    <row r="932" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A932" s="7"/>
-      <c r="B932" s="7"/>
-    </row>
-    <row r="933" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A933" s="7"/>
-      <c r="B933" s="7"/>
-    </row>
-    <row r="934" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A934" s="7"/>
-      <c r="B934" s="7"/>
-    </row>
-    <row r="935" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A935" s="7"/>
-      <c r="B935" s="7"/>
-    </row>
-    <row r="936" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A936" s="7"/>
-      <c r="B936" s="7"/>
-    </row>
-    <row r="937" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A937" s="7"/>
-      <c r="B937" s="7"/>
-    </row>
-    <row r="938" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A938" s="7"/>
-      <c r="B938" s="7"/>
-    </row>
-    <row r="939" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A939" s="7"/>
-      <c r="B939" s="7"/>
-    </row>
-    <row r="940" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A940" s="7"/>
-      <c r="B940" s="7"/>
-    </row>
-    <row r="941" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A941" s="7"/>
-      <c r="B941" s="7"/>
-    </row>
-    <row r="942" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A942" s="7"/>
-      <c r="B942" s="7"/>
-    </row>
-    <row r="943" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A943" s="7"/>
-      <c r="B943" s="7"/>
-    </row>
-    <row r="944" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A944" s="7"/>
-      <c r="B944" s="7"/>
-    </row>
-    <row r="945" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A945" s="7"/>
-      <c r="B945" s="7"/>
-    </row>
-    <row r="946" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A946" s="7"/>
-      <c r="B946" s="7"/>
-    </row>
-    <row r="947" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A947" s="7"/>
-      <c r="B947" s="7"/>
-    </row>
-    <row r="948" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A948" s="7"/>
-      <c r="B948" s="7"/>
-    </row>
-    <row r="949" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A949" s="7"/>
-      <c r="B949" s="7"/>
-    </row>
-    <row r="950" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A950" s="7"/>
-      <c r="B950" s="7"/>
-    </row>
-    <row r="951" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A951" s="7"/>
-      <c r="B951" s="7"/>
-    </row>
-    <row r="952" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A952" s="7"/>
-      <c r="B952" s="7"/>
-    </row>
-    <row r="953" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A953" s="7"/>
-      <c r="B953" s="7"/>
-    </row>
-    <row r="954" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A954" s="7"/>
-      <c r="B954" s="7"/>
-    </row>
-    <row r="955" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A955" s="7"/>
-      <c r="B955" s="7"/>
-    </row>
-    <row r="956" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A956" s="7"/>
-      <c r="B956" s="7"/>
-    </row>
-    <row r="957" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A957" s="7"/>
-      <c r="B957" s="7"/>
-    </row>
-    <row r="958" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A958" s="7"/>
-      <c r="B958" s="7"/>
-    </row>
-    <row r="959" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A959" s="7"/>
-      <c r="B959" s="7"/>
-    </row>
-    <row r="960" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A960" s="7"/>
-      <c r="B960" s="7"/>
-    </row>
-    <row r="961" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A961" s="7"/>
-      <c r="B961" s="7"/>
-    </row>
-    <row r="962" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A962" s="7"/>
-      <c r="B962" s="7"/>
-    </row>
-    <row r="963" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A963" s="7"/>
-      <c r="B963" s="7"/>
-    </row>
-    <row r="964" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A964" s="7"/>
-      <c r="B964" s="7"/>
-    </row>
-    <row r="965" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A965" s="7"/>
-      <c r="B965" s="7"/>
-    </row>
-    <row r="966" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A966" s="7"/>
-      <c r="B966" s="7"/>
-    </row>
-    <row r="967" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A967" s="7"/>
-      <c r="B967" s="7"/>
-    </row>
-    <row r="968" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A968" s="7"/>
-      <c r="B968" s="7"/>
-    </row>
-    <row r="969" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A969" s="7"/>
-      <c r="B969" s="7"/>
-    </row>
-    <row r="970" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A970" s="7"/>
-      <c r="B970" s="7"/>
-    </row>
-    <row r="971" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A971" s="7"/>
-      <c r="B971" s="7"/>
-    </row>
-    <row r="972" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A972" s="7"/>
-      <c r="B972" s="7"/>
-    </row>
-    <row r="973" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A973" s="7"/>
-      <c r="B973" s="7"/>
-    </row>
-    <row r="974" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A974" s="7"/>
-      <c r="B974" s="7"/>
-    </row>
-    <row r="975" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A975" s="7"/>
-      <c r="B975" s="7"/>
-    </row>
-    <row r="976" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A976" s="7"/>
-      <c r="B976" s="7"/>
-    </row>
-    <row r="977" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A977" s="7"/>
-      <c r="B977" s="7"/>
-    </row>
-    <row r="978" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A978" s="7"/>
-      <c r="B978" s="7"/>
-    </row>
-    <row r="979" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A979" s="7"/>
-      <c r="B979" s="7"/>
-    </row>
-    <row r="980" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A980" s="7"/>
-      <c r="B980" s="7"/>
-    </row>
-    <row r="981" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A981" s="7"/>
-      <c r="B981" s="7"/>
-    </row>
-    <row r="982" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A982" s="7"/>
-      <c r="B982" s="7"/>
-    </row>
-    <row r="983" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A983" s="7"/>
-      <c r="B983" s="7"/>
-    </row>
-    <row r="984" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A984" s="7"/>
-      <c r="B984" s="7"/>
-    </row>
-    <row r="985" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A985" s="7"/>
-      <c r="B985" s="7"/>
-    </row>
-    <row r="986" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A986" s="7"/>
-      <c r="B986" s="7"/>
-    </row>
-    <row r="987" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A987" s="7"/>
-      <c r="B987" s="7"/>
-    </row>
-    <row r="988" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A988" s="7"/>
-      <c r="B988" s="7"/>
-    </row>
-    <row r="989" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A989" s="7"/>
-      <c r="B989" s="7"/>
-    </row>
-    <row r="990" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A990" s="7"/>
-      <c r="B990" s="7"/>
-    </row>
-    <row r="991" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A991" s="7"/>
-      <c r="B991" s="7"/>
-    </row>
-    <row r="992" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A992" s="7"/>
-      <c r="B992" s="7"/>
-    </row>
-    <row r="993" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A993" s="7"/>
-      <c r="B993" s="7"/>
-    </row>
-    <row r="994" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A994" s="7"/>
-      <c r="B994" s="7"/>
-    </row>
-    <row r="995" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A995" s="7"/>
-      <c r="B995" s="7"/>
-    </row>
-    <row r="996" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A996" s="7"/>
-      <c r="B996" s="7"/>
-    </row>
-    <row r="997" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A997" s="7"/>
-      <c r="B997" s="7"/>
-    </row>
-    <row r="998" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A998" s="7"/>
-      <c r="B998" s="7"/>
-    </row>
-    <row r="999" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A999" s="7"/>
-      <c r="B999" s="7"/>
-    </row>
-    <row r="1000" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1000" s="7"/>
-      <c r="B1000" s="7"/>
-    </row>
-    <row r="1001" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1001" s="7"/>
-      <c r="B1001" s="7"/>
-    </row>
-    <row r="1002" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1002" s="7"/>
-      <c r="B1002" s="7"/>
-    </row>
-    <row r="1003" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1003" s="7"/>
-      <c r="B1003" s="7"/>
-    </row>
-    <row r="1004" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1004" s="7"/>
-      <c r="B1004" s="7"/>
-    </row>
-    <row r="1005" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1005" s="7"/>
-      <c r="B1005" s="7"/>
-    </row>
-    <row r="1006" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1006" s="7"/>
-      <c r="B1006" s="7"/>
-    </row>
-    <row r="1007" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1007" s="7"/>
-      <c r="B1007" s="7"/>
-    </row>
-    <row r="1008" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1008" s="7"/>
-      <c r="B1008" s="7"/>
-    </row>
-    <row r="1009" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1009" s="7"/>
-      <c r="B1009" s="7"/>
-    </row>
-    <row r="1010" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1010" s="7"/>
-      <c r="B1010" s="7"/>
-    </row>
-    <row r="1011" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1011" s="7"/>
-      <c r="B1011" s="7"/>
-    </row>
-    <row r="1012" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1012" s="7"/>
-      <c r="B1012" s="7"/>
-    </row>
-    <row r="1013" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1013" s="7"/>
-      <c r="B1013" s="7"/>
-    </row>
-    <row r="1014" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1014" s="7"/>
-      <c r="B1014" s="7"/>
-    </row>
-    <row r="1015" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1015" s="7"/>
-      <c r="B1015" s="7"/>
-    </row>
-    <row r="1016" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1016" s="7"/>
-      <c r="B1016" s="7"/>
-    </row>
-    <row r="1017" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1017" s="7"/>
-      <c r="B1017" s="7"/>
-    </row>
-    <row r="1018" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1018" s="7"/>
-      <c r="B1018" s="7"/>
-    </row>
-    <row r="1019" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1019" s="7"/>
-      <c r="B1019" s="7"/>
-    </row>
-    <row r="1020" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1020" s="7"/>
-      <c r="B1020" s="7"/>
-    </row>
-    <row r="1021" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1021" s="7"/>
-      <c r="B1021" s="7"/>
-    </row>
-    <row r="1022" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1022" s="7"/>
-      <c r="B1022" s="7"/>
-    </row>
-    <row r="1023" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1023" s="7"/>
-      <c r="B1023" s="7"/>
-    </row>
-    <row r="1024" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1024" s="7"/>
-      <c r="B1024" s="7"/>
-    </row>
-    <row r="1025" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1025" s="7"/>
-      <c r="B1025" s="7"/>
-    </row>
-    <row r="1026" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1026" s="7"/>
-      <c r="B1026" s="7"/>
-    </row>
-    <row r="1027" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1027" s="7"/>
-      <c r="B1027" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -19540,7 +18016,7 @@
     <mergeCell ref="G3:G8"/>
     <mergeCell ref="G9:G25"/>
   </mergeCells>
-  <conditionalFormatting sqref="H55:H1048576 H1:H15 H18:H41 H44:H50">
+  <conditionalFormatting sqref="H1:H15 H18:H41 H44:H50 H55:H1048576">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
@@ -19566,7 +18042,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E57:E227 E3:E54" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E57:E125 E3:E54" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Critical,High,Low"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updating/Debugging of editBidProcess.php and processBid.php
Co-Authored-By: lifuhuang97 <lifuhuang97@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YL\Desktop\SMU YEAR 2\Y2S1\Software Project Management G8 IS212\SPM\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9478AB50-2C4D-451B-A847-B6D6F6EF1D94}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E545853E-DD4F-4802-AA2E-15912CF475FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="110">
   <si>
     <t>Severity</t>
   </si>
@@ -355,6 +355,12 @@
   <si>
     <t>Failure to check when user enter a value that have more than 2 decimal.</t>
   </si>
+  <si>
+    <t>Add Bid process, Edit bid process</t>
+  </si>
+  <si>
+    <t>Failure to check when user enter a value high than his/her edollars</t>
+  </si>
 </sst>
 </file>
 
@@ -654,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -881,9 +887,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1460,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1478,16 +1481,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
     </row>
     <row r="2" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
@@ -2563,7 +2566,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A39" s="41">
         <v>37</v>
       </c>
@@ -2787,7 +2790,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A47" s="41">
         <v>45</v>
       </c>
@@ -2814,7 +2817,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="41">
         <v>46</v>
       </c>
@@ -2823,7 +2826,7 @@
       </c>
       <c r="C48" s="41" t="str">
         <f>'Bug Metrics'!$C48</f>
-        <v>Add Bid</v>
+        <v>Add Bid process, Edit bid process</v>
       </c>
       <c r="D48" s="75" t="s">
         <v>107</v>
@@ -2841,15 +2844,32 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="41"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="77"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="44"/>
-      <c r="H49" s="45"/>
+    <row r="49" spans="1:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="41">
+        <v>47</v>
+      </c>
+      <c r="B49" s="41">
+        <v>4</v>
+      </c>
+      <c r="C49" s="41" t="str">
+        <f>'Bug Metrics'!$C49</f>
+        <v>Add Bid process, Edit bid process</v>
+      </c>
+      <c r="D49" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F49" s="44">
+        <v>43777</v>
+      </c>
+      <c r="G49" s="44">
+        <v>43779</v>
+      </c>
+      <c r="H49" s="45" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="41"/>
@@ -12455,7 +12475,7 @@
   <dimension ref="A1:H925"/>
   <sheetViews>
     <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49:F49"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12472,16 +12492,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
@@ -12530,7 +12550,7 @@
         <f t="shared" ref="F3:F125" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G3" s="84">
+      <c r="G3" s="83">
         <f>SUM($F3:$F8)</f>
         <v>27</v>
       </c>
@@ -12560,7 +12580,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="81"/>
+      <c r="G4" s="80"/>
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -12584,7 +12604,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="81"/>
+      <c r="G5" s="80"/>
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -12608,7 +12628,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G6" s="81"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -12632,7 +12652,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G7" s="81"/>
+      <c r="G7" s="80"/>
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -12656,7 +12676,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G8" s="85"/>
+      <c r="G8" s="84"/>
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12680,7 +12700,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G9" s="84">
+      <c r="G9" s="83">
         <f>SUM(F9:F25)</f>
         <v>87</v>
       </c>
@@ -12710,7 +12730,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G10" s="81"/>
+      <c r="G10" s="80"/>
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -12734,7 +12754,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G11" s="81"/>
+      <c r="G11" s="80"/>
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -12758,7 +12778,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="81"/>
+      <c r="G12" s="80"/>
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -12782,7 +12802,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G13" s="81"/>
+      <c r="G13" s="80"/>
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -12806,7 +12826,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G14" s="81"/>
+      <c r="G14" s="80"/>
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -12830,7 +12850,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G15" s="81"/>
+      <c r="G15" s="80"/>
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -12854,7 +12874,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G16" s="81"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -12878,7 +12898,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G17" s="81"/>
+      <c r="G17" s="80"/>
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -12902,7 +12922,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G18" s="81"/>
+      <c r="G18" s="80"/>
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -12926,7 +12946,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G19" s="81"/>
+      <c r="G19" s="80"/>
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -12950,7 +12970,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G20" s="81"/>
+      <c r="G20" s="80"/>
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -12974,7 +12994,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G21" s="81"/>
+      <c r="G21" s="80"/>
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -12998,7 +13018,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G22" s="81"/>
+      <c r="G22" s="80"/>
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -13022,7 +13042,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G23" s="81"/>
+      <c r="G23" s="80"/>
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -13046,7 +13066,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G24" s="81"/>
+      <c r="G24" s="80"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -13070,7 +13090,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G25" s="81"/>
+      <c r="G25" s="80"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13094,7 +13114,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G26" s="83">
+      <c r="G26" s="82">
         <f>SUM(F26:F43)</f>
         <v>67</v>
       </c>
@@ -13124,7 +13144,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G27" s="81"/>
+      <c r="G27" s="80"/>
       <c r="H27" s="63"/>
     </row>
     <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -13148,7 +13168,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G28" s="81"/>
+      <c r="G28" s="80"/>
       <c r="H28" s="63"/>
     </row>
     <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -13172,7 +13192,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G29" s="81"/>
+      <c r="G29" s="80"/>
       <c r="H29" s="63"/>
     </row>
     <row r="30" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -13196,7 +13216,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G30" s="81"/>
+      <c r="G30" s="80"/>
       <c r="H30" s="63"/>
     </row>
     <row r="31" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -13220,7 +13240,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G31" s="81"/>
+      <c r="G31" s="80"/>
       <c r="H31" s="63"/>
     </row>
     <row r="32" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -13244,7 +13264,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G32" s="81"/>
+      <c r="G32" s="80"/>
       <c r="H32" s="63"/>
     </row>
     <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -13268,7 +13288,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G33" s="81"/>
+      <c r="G33" s="80"/>
       <c r="H33" s="63"/>
     </row>
     <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -13292,7 +13312,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G34" s="81"/>
+      <c r="G34" s="80"/>
       <c r="H34" s="63"/>
     </row>
     <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -13316,7 +13336,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G35" s="81"/>
+      <c r="G35" s="80"/>
       <c r="H35" s="63"/>
     </row>
     <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -13340,7 +13360,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G36" s="81"/>
+      <c r="G36" s="80"/>
       <c r="H36" s="63"/>
     </row>
     <row r="37" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -13364,7 +13384,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G37" s="81"/>
+      <c r="G37" s="80"/>
       <c r="H37" s="63"/>
     </row>
     <row r="38" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -13388,7 +13408,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G38" s="81"/>
+      <c r="G38" s="80"/>
       <c r="H38" s="63"/>
     </row>
     <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -13412,7 +13432,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G39" s="81"/>
+      <c r="G39" s="80"/>
       <c r="H39" s="63"/>
     </row>
     <row r="40" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -13435,7 +13455,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G40" s="81"/>
+      <c r="G40" s="80"/>
       <c r="H40" s="63"/>
     </row>
     <row r="41" spans="1:8" s="56" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
@@ -13458,7 +13478,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G41" s="81"/>
+      <c r="G41" s="80"/>
       <c r="H41" s="63"/>
     </row>
     <row r="42" spans="1:8" s="56" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
@@ -13482,7 +13502,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G42" s="81"/>
+      <c r="G42" s="80"/>
       <c r="H42" s="63"/>
     </row>
     <row r="43" spans="1:8" s="56" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -13506,7 +13526,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G43" s="82"/>
+      <c r="G43" s="81"/>
       <c r="H43" s="64"/>
     </row>
     <row r="44" spans="1:8" s="56" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13530,9 +13550,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G44" s="83">
+      <c r="G44" s="82">
         <f>SUM(F44:F50)</f>
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H44" s="70" t="str">
         <f xml:space="preserve"> IF(G44&lt;10,Instructions!B7,Instructions!B8)</f>
@@ -13560,7 +13580,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G45" s="81"/>
+      <c r="G45" s="80"/>
       <c r="H45" s="63"/>
     </row>
     <row r="46" spans="1:8" s="56" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13584,7 +13604,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G46" s="81"/>
+      <c r="G46" s="80"/>
       <c r="H46" s="63"/>
     </row>
     <row r="47" spans="1:8" s="56" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13608,10 +13628,10 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G47" s="81"/>
+      <c r="G47" s="80"/>
       <c r="H47" s="63"/>
     </row>
-    <row r="48" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A48" s="71">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -13620,7 +13640,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="D48" s="24" t="s">
         <v>107</v>
@@ -13632,10 +13652,10 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G48" s="81"/>
+      <c r="G48" s="80"/>
       <c r="H48" s="63"/>
     </row>
-    <row r="49" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A49" s="71">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -13643,11 +13663,20 @@
       <c r="B49" s="12">
         <v>4</v>
       </c>
-      <c r="C49" s="27"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="76"/>
-      <c r="F49" s="76"/>
-      <c r="G49" s="81"/>
+      <c r="C49" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E49" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="F49" s="76">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G49" s="80"/>
       <c r="H49" s="63"/>
     </row>
     <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -13665,7 +13694,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G50" s="82"/>
+      <c r="G50" s="81"/>
       <c r="H50" s="64"/>
     </row>
     <row r="51" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13683,7 +13712,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G51" s="81">
+      <c r="G51" s="80">
         <f>SUM(F51:F54)</f>
         <v>0</v>
       </c>
@@ -13707,7 +13736,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G52" s="81"/>
+      <c r="G52" s="80"/>
       <c r="H52" s="63"/>
     </row>
     <row r="53" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -13725,7 +13754,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G53" s="81"/>
+      <c r="G53" s="80"/>
       <c r="H53" s="63"/>
     </row>
     <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -13743,7 +13772,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G54" s="82"/>
+      <c r="G54" s="81"/>
       <c r="H54" s="64"/>
     </row>
     <row r="55" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Debug for bid status
Co-Authored-By: tvngo2018 <tvngo2018@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YL\Desktop\SMU YEAR 2\Y2S1\Software Project Management G8 IS212\SPM\project-g8t9\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tee-y\Desktop\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E545853E-DD4F-4802-AA2E-15912CF475FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A2BE05-BAF4-419D-98EB-CB791F73F2A3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="113">
   <si>
     <t>Severity</t>
   </si>
@@ -360,6 +360,15 @@
   </si>
   <si>
     <t>Failure to check when user enter a value high than his/her edollars</t>
+  </si>
+  <si>
+    <t>Bid Status</t>
+  </si>
+  <si>
+    <t>Wrong students display order</t>
+  </si>
+  <si>
+    <t>TY &amp; C</t>
   </si>
 </sst>
 </file>
@@ -1463,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2872,14 +2881,32 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="41"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="45"/>
+      <c r="A50" s="41">
+        <v>48</v>
+      </c>
+      <c r="B50" s="41">
+        <v>5</v>
+      </c>
+      <c r="C50" s="41" t="str">
+        <f>'Bug Metrics'!C51</f>
+        <v>Bid Status</v>
+      </c>
+      <c r="D50" s="29" t="str">
+        <f>'Bug Metrics'!D51</f>
+        <v>Wrong students display order</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="44">
+        <v>43785</v>
+      </c>
+      <c r="G50" s="44">
+        <v>43785</v>
+      </c>
+      <c r="H50" s="45" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="41"/>
@@ -12474,8 +12501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H925"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13705,16 +13732,22 @@
       <c r="B51" s="12">
         <v>5</v>
       </c>
-      <c r="C51" s="27"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54" t="str">
+      <c r="C51" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="F51" s="54">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G51" s="80">
         <f>SUM(F51:F54)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" s="63" t="str">
         <f xml:space="preserve"> IF(G51&lt;10,Instructions!B7,Instructions!B8)</f>

</xml_diff>

<commit_message>
Debug for JSON decimal value display format
Co-Authored-By: tvngo2018 <tvngo2018@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tee-y\Desktop\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A2BE05-BAF4-419D-98EB-CB791F73F2A3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307B63AE-9837-45F8-BA1E-A53E23DBAC0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7548" yWindow="444" windowWidth="13008" windowHeight="11916" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="115">
   <si>
     <t>Severity</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t>TY &amp; C</t>
+  </si>
+  <si>
+    <t>Bid-dump, bid-status, dump, section-dump, user-dump</t>
+  </si>
+  <si>
+    <t>Wrong display of decimal place for json message</t>
   </si>
 </sst>
 </file>
@@ -1472,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="D28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51:H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2909,14 +2915,32 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="41"/>
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="45"/>
+      <c r="A51" s="41">
+        <v>49</v>
+      </c>
+      <c r="B51" s="41">
+        <v>5</v>
+      </c>
+      <c r="C51" s="41" t="str">
+        <f>'Bug Metrics'!C52</f>
+        <v>Bid-dump, bid-status, dump, section-dump, user-dump</v>
+      </c>
+      <c r="D51" s="41" t="str">
+        <f>'Bug Metrics'!D52</f>
+        <v>Wrong display of decimal place for json message</v>
+      </c>
+      <c r="E51" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="44">
+        <v>43785</v>
+      </c>
+      <c r="G51" s="44">
+        <v>43785</v>
+      </c>
+      <c r="H51" s="45" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="41"/>
@@ -12502,7 +12526,7 @@
   <dimension ref="A1:H925"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13754,7 +13778,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A52" s="71">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -13762,8 +13786,12 @@
       <c r="B52" s="12">
         <v>5</v>
       </c>
-      <c r="C52" s="27"/>
-      <c r="D52" s="24"/>
+      <c r="C52" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>114</v>
+      </c>
       <c r="E52" s="54"/>
       <c r="F52" s="54" t="str">
         <f t="shared" si="0"/>

</xml_diff>